<commit_message>
entire code is updated
</commit_message>
<xml_diff>
--- a/TestData/OrbitScience_data.xlsx
+++ b/TestData/OrbitScience_data.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Smoke" sheetId="1" r:id="rId1"/>
     <sheet name="Regression" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="92">
   <si>
     <t>#</t>
   </si>
@@ -55,18 +56,9 @@
     <t>TC003_addMainCategory</t>
   </si>
   <si>
-    <t>LC-MS Solvents</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>C:\\Users\\Chaitanya\\Desktop\\Project details\\Sample images\\bencodryl-sf-500x500.jpg</t>
   </si>
   <si>
-    <t>Bcetone</t>
-  </si>
-  <si>
     <t>TC004_addMainCategoryDuplicateRecord</t>
   </si>
   <si>
@@ -79,9 +71,6 @@
     <t>TC006_editMainCategory</t>
   </si>
   <si>
-    <t>chlorine</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -94,12 +83,6 @@
     <t>TC008_addSubCategory</t>
   </si>
   <si>
-    <t>Paractmal</t>
-  </si>
-  <si>
-    <t>Headace</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -115,9 +98,6 @@
     <t>TC011_editSubCategory</t>
   </si>
   <si>
-    <t>PainKiller</t>
-  </si>
-  <si>
     <t>TC0012_deleteSubCategory</t>
   </si>
   <si>
@@ -139,15 +119,9 @@
     <t>TC0019_deleteProduct</t>
   </si>
   <si>
-    <t>cat123</t>
-  </si>
-  <si>
     <t>TC020_homePage</t>
   </si>
   <si>
-    <t>chemical</t>
-  </si>
-  <si>
     <t>TC021_searchWithoutInputTheData</t>
   </si>
   <si>
@@ -160,15 +134,9 @@
     <t>TC023_searchWithProductName</t>
   </si>
   <si>
-    <t>123D1</t>
-  </si>
-  <si>
     <t>TC024_searchWithSynonym</t>
   </si>
   <si>
-    <t>Tyl</t>
-  </si>
-  <si>
     <t>TC025_searchWithCatNo</t>
   </si>
   <si>
@@ -221,13 +189,133 @@
   </si>
   <si>
     <t>TC006_editProducts</t>
+  </si>
+  <si>
+    <t>GC-MS Slovents</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>GC-MS Slovents(Gas-Mass)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Defect description</t>
+  </si>
+  <si>
+    <t>image is not selecting</t>
+  </si>
+  <si>
+    <t>image is not selecting and documents also not able to upload</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>cronic</t>
+  </si>
+  <si>
+    <t>GC-HS Slovents</t>
+  </si>
+  <si>
+    <t>GC-HS Slovents(Diluents)</t>
+  </si>
+  <si>
+    <t>cropol-500</t>
+  </si>
+  <si>
+    <t>SU01651000</t>
+  </si>
+  <si>
+    <t>Dimethyl sulfoxide</t>
+  </si>
+  <si>
+    <t>&gt; 99,99 %</t>
+  </si>
+  <si>
+    <t>DMSO</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF4D4D4D"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>67-68-5</t>
+    </r>
+  </si>
+  <si>
+    <t>Scharlau, Spain</t>
+  </si>
+  <si>
+    <t>1 Litre</t>
+  </si>
+  <si>
+    <t>Hs123</t>
+  </si>
+  <si>
+    <t>&gt;98</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>2liters</t>
+  </si>
+  <si>
+    <t>CH123</t>
+  </si>
+  <si>
+    <t>HS456</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>folic acid</t>
+  </si>
+  <si>
+    <t>12cc</t>
+  </si>
+  <si>
+    <t>Scharlau</t>
+  </si>
+  <si>
+    <t>6Litre</t>
+  </si>
+  <si>
+    <t>Lot no is not taking</t>
+  </si>
+  <si>
+    <t>documents is not able to upload</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +363,31 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF484343"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4D4D4D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -318,15 +431,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -336,6 +446,12 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -656,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -665,16 +781,16 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -682,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -691,13 +807,13 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -705,7 +821,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -719,7 +835,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -733,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -747,7 +863,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -794,10 +910,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,13 +921,14 @@
     <col min="2" max="2" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -825,7 +942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -839,7 +956,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -850,7 +970,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -861,421 +984,630 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="H4" t="s">
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N14">
+        <v>19</v>
+      </c>
+      <c r="O14" t="s">
+        <v>78</v>
+      </c>
+      <c r="P14">
+        <v>6800</v>
+      </c>
+      <c r="Q14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="R14" t="s">
+        <v>57</v>
+      </c>
+      <c r="S14" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I15">
+        <v>100</v>
+      </c>
+      <c r="J15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L15" t="s">
+        <v>85</v>
+      </c>
+      <c r="M15" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M16">
+        <v>19</v>
+      </c>
+      <c r="N16" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16">
+        <v>6800</v>
+      </c>
+      <c r="P16" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>57</v>
+      </c>
+      <c r="R16" t="s">
+        <v>57</v>
+      </c>
+      <c r="S16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17">
+        <v>19</v>
+      </c>
+      <c r="O17" t="s">
+        <v>78</v>
+      </c>
+      <c r="P17">
+        <v>6800</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>14</v>
+      </c>
+      <c r="R17" t="s">
+        <v>57</v>
+      </c>
+      <c r="S17" t="s">
+        <v>57</v>
+      </c>
+      <c r="T17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18">
+        <v>50</v>
+      </c>
+      <c r="K18">
+        <v>7800</v>
+      </c>
+      <c r="L18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>20</v>
       </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-      <c r="I7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>22</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>24</v>
       </c>
-      <c r="F9" t="s">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>25</v>
       </c>
-      <c r="G9" t="s">
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>26</v>
       </c>
-      <c r="H9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="B28" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="6">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="5">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="5">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="51.75" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" s="7">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="8">
+      <c r="D30" s="7">
         <v>777</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1283,5 +1615,372 @@
     <hyperlink ref="D3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>